<commit_message>
adding the invmenet file to the git repository
</commit_message>
<xml_diff>
--- a/Investement/Balance Track.xlsx
+++ b/Investement/Balance Track.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Investement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gamerFun\Investement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F5E6160-9D8D-419D-B394-66725072D16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C341D431-1927-4731-B6D4-5BB3DB96D042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{9373AB9F-C255-43C0-9C0B-0B022A757888}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Total balance </t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>3,928.10 Euro</t>
+  </si>
+  <si>
+    <t>4007.37 Euro</t>
   </si>
 </sst>
 </file>
@@ -94,10 +97,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FC221F-C60B-430F-A66D-4F292047634D}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -460,6 +466,14 @@
         <v>45456</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45463</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>